<commit_message>
Recalculate mean success rate and mean number of grammar changes
</commit_message>
<xml_diff>
--- a/results/compare_num_of_changes.xlsx
+++ b/results/compare_num_of_changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\esjou\Dropbox\linguist\Jou\Generals\Generals02\code\economy_RIPGLA\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\linguist\Jou\projects\2021_RIP\Generals02\code\economy_RIPGLA\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63A1A9-1E0B-4406-B17F-77427C1FA7F0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD74FB46-EDDA-4593-9FDD-8C58D6CBBAA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nonnoisy_changeinfo_original" sheetId="1" r:id="rId1"/>
@@ -25,13 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="80">
-  <si>
-    <t>hypo01</t>
-  </si>
-  <si>
-    <t>hypo02</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
   <si>
     <t>hypo03</t>
   </si>
@@ -283,7 +277,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1231,1765 +1225,1720 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" t="s">
         <v>68</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>69</v>
       </c>
-      <c r="C1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>1279</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="D2" t="str">
-        <f>IF(B2&lt;C2,"OT","ERC")</f>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" ref="D2:D64" si="0">IF(B2&lt;C2,"OT","ERC")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1279</v>
+        <v>160</v>
       </c>
       <c r="C3">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D66" si="0">IF(B3&lt;C3,"OT","ERC")</f>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>241</v>
+      </c>
+      <c r="C4">
+        <v>153</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>160</v>
-      </c>
-      <c r="C4">
-        <v>158</v>
-      </c>
-      <c r="D4" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
       <c r="B5">
-        <v>241</v>
+        <v>189.5</v>
       </c>
       <c r="C5">
-        <v>153</v>
+        <v>187.5</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>189.5</v>
+        <v>141</v>
       </c>
       <c r="C6">
-        <v>187.5</v>
+        <v>133.5</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>97</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>141</v>
-      </c>
-      <c r="C7">
-        <v>133.5</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+      <c r="B8">
+        <v>131</v>
+      </c>
+      <c r="C8">
+        <v>89</v>
+      </c>
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>105</v>
-      </c>
-      <c r="C8">
-        <v>97</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
       <c r="B9">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="C9">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D9" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>3500</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>3500</v>
+        <v>53</v>
       </c>
       <c r="C12">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>146.5</v>
+      </c>
+      <c r="C13">
+        <v>90.5</v>
+      </c>
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>53</v>
-      </c>
-      <c r="C13">
-        <v>51</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>146.5</v>
-      </c>
-      <c r="C14">
-        <v>90.5</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>170</v>
+      </c>
+      <c r="C15">
+        <v>107</v>
+      </c>
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B16">
+        <v>5478</v>
+      </c>
+      <c r="C16">
+        <v>159</v>
+      </c>
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="C15">
-        <v>19</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>170</v>
-      </c>
-      <c r="C16">
-        <v>107</v>
-      </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
       <c r="B17">
-        <v>5478</v>
+        <v>5348.5</v>
       </c>
       <c r="C17">
-        <v>159</v>
+        <v>39</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
-        <v>5348.5</v>
+        <v>93</v>
       </c>
       <c r="C18">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>16.5</v>
       </c>
       <c r="C19">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16.5</v>
+        <v>954</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>189.5</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>954</v>
+        <v>3061</v>
       </c>
       <c r="C21">
-        <v>189.5</v>
+        <v>106.5</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>3061</v>
+        <v>132</v>
       </c>
       <c r="C22">
-        <v>106.5</v>
+        <v>129</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>132</v>
+        <v>5426</v>
       </c>
       <c r="C23">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>5426</v>
+        <v>1729</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>1729</v>
+        <v>2915</v>
       </c>
       <c r="C25">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>2915</v>
+        <v>451.5</v>
       </c>
       <c r="C26">
-        <v>157</v>
+        <v>43</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>451.5</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>43</v>
+        <v>49.5</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>41</v>
       </c>
       <c r="B28">
-        <v>50</v>
+        <v>9723</v>
       </c>
       <c r="C28">
-        <v>49.5</v>
+        <v>44</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>97.5</v>
+      </c>
+      <c r="C29">
+        <v>97</v>
+      </c>
+      <c r="D29" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
-        <v>9723</v>
-      </c>
-      <c r="C29">
-        <v>44</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
       <c r="B30">
-        <v>97.5</v>
+        <v>90</v>
       </c>
       <c r="C30">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>45</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="C31">
-        <v>86</v>
+        <v>229.5</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>2963</v>
+      </c>
+      <c r="C32">
+        <v>103</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B32">
-        <v>248</v>
-      </c>
-      <c r="C32">
-        <v>229.5</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B33">
+        <v>96</v>
+      </c>
+      <c r="C33">
+        <v>91</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B33">
-        <v>2963</v>
-      </c>
-      <c r="C33">
-        <v>103</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B34">
+        <v>51.5</v>
+      </c>
+      <c r="C34">
         <v>49</v>
       </c>
-      <c r="B34">
-        <v>96</v>
-      </c>
-      <c r="C34">
-        <v>91</v>
-      </c>
       <c r="D34" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>51.5</v>
+        <v>274</v>
       </c>
       <c r="C35">
-        <v>49</v>
+        <v>104.5</v>
       </c>
       <c r="D35" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>51</v>
       </c>
       <c r="B36">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C36">
-        <v>104.5</v>
+        <v>88</v>
       </c>
       <c r="D36" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
-        <v>280</v>
+        <v>231</v>
       </c>
       <c r="C37">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D37" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>54</v>
       </c>
       <c r="B38">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="C38">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="D38" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>232</v>
+      </c>
+      <c r="C39">
+        <v>221.5</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>56</v>
       </c>
-      <c r="B39">
-        <v>184</v>
-      </c>
-      <c r="C39">
-        <v>168</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
       <c r="B40">
-        <v>232</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>221.5</v>
+        <v>19</v>
       </c>
       <c r="D40" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D41" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>141</v>
+      </c>
+      <c r="C42">
+        <v>129</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>61</v>
       </c>
-      <c r="B42">
-        <v>223</v>
-      </c>
-      <c r="C42">
-        <v>214</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>62</v>
-      </c>
       <c r="B43">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C43">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="D43" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B44">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C44">
-        <v>100</v>
+        <v>118.5</v>
       </c>
       <c r="D44" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45">
-        <v>119</v>
+        <v>414</v>
       </c>
       <c r="C45">
-        <v>118.5</v>
+        <v>147</v>
       </c>
       <c r="D45" t="str">
         <f t="shared" si="0"/>
         <v>ERC</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:4">
       <c r="A46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46">
-        <v>414</v>
+        <v>10</v>
+      </c>
+      <c r="B46" t="s">
+        <v>77</v>
       </c>
       <c r="C46">
+        <v>91</v>
+      </c>
+      <c r="D46" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" t="s">
+        <v>31</v>
+      </c>
+      <c r="B47" t="s">
+        <v>77</v>
+      </c>
+      <c r="C47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>1</v>
+      </c>
+      <c r="B49">
         <v>147</v>
       </c>
-      <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>12</v>
-      </c>
-      <c r="B47" t="s">
-        <v>79</v>
-      </c>
-      <c r="C47">
-        <v>91</v>
-      </c>
-      <c r="D47" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" t="s">
-        <v>79</v>
-      </c>
-      <c r="C48" t="s">
-        <v>79</v>
-      </c>
-      <c r="D48" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A49" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" t="s">
-        <v>79</v>
-      </c>
-      <c r="C49" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C49">
+        <v>159</v>
+      </c>
+      <c r="D49" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B50">
         <v>82.5</v>
       </c>
       <c r="C50">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D50" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:4">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B51">
-        <v>147</v>
+        <v>187</v>
       </c>
       <c r="C51">
-        <v>159</v>
+        <v>198.5</v>
       </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:4">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B52">
-        <v>82.5</v>
+        <v>130</v>
       </c>
       <c r="C52">
-        <v>84</v>
+        <v>180</v>
       </c>
       <c r="D52" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:4">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B53">
-        <v>187</v>
+        <v>50</v>
       </c>
       <c r="C53">
-        <v>198.5</v>
+        <v>52</v>
       </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:4">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B54">
-        <v>130</v>
+        <v>177</v>
       </c>
       <c r="C54">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:4">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B55">
+        <v>115</v>
+      </c>
+      <c r="C55">
+        <v>122</v>
+      </c>
+      <c r="D55" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" t="s">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>133.5</v>
+      </c>
+      <c r="C56">
+        <v>146</v>
+      </c>
+      <c r="D56" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" t="s">
+        <v>33</v>
+      </c>
+      <c r="B57">
+        <v>63</v>
+      </c>
+      <c r="C57">
+        <v>67.5</v>
+      </c>
+      <c r="D57" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58">
+        <v>62</v>
+      </c>
+      <c r="C58">
+        <v>68</v>
+      </c>
+      <c r="D58" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59">
+        <v>62.5</v>
+      </c>
+      <c r="C59">
+        <v>63</v>
+      </c>
+      <c r="D59" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" t="s">
+        <v>40</v>
+      </c>
+      <c r="B60">
+        <v>145</v>
+      </c>
+      <c r="C60">
+        <v>155</v>
+      </c>
+      <c r="D60" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" t="s">
+        <v>44</v>
+      </c>
+      <c r="B61">
+        <v>89</v>
+      </c>
+      <c r="C61">
+        <v>102</v>
+      </c>
+      <c r="D61" t="str">
+        <f t="shared" si="0"/>
+        <v>OT</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" t="s">
         <v>50</v>
       </c>
-      <c r="C55">
-        <v>52</v>
-      </c>
-      <c r="D55" t="str">
+      <c r="B62">
+        <v>142.5</v>
+      </c>
+      <c r="C62">
+        <v>151.5</v>
+      </c>
+      <c r="D62" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A56" t="s">
-        <v>27</v>
-      </c>
-      <c r="B56">
-        <v>177</v>
-      </c>
-      <c r="C56">
-        <v>184</v>
-      </c>
-      <c r="D56" t="str">
+    <row r="63" spans="1:4">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63">
+        <v>75</v>
+      </c>
+      <c r="C63">
+        <v>79</v>
+      </c>
+      <c r="D63" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A57" t="s">
-        <v>29</v>
-      </c>
-      <c r="B57">
-        <v>115</v>
-      </c>
-      <c r="C57">
-        <v>122</v>
-      </c>
-      <c r="D57" t="str">
+    <row r="64" spans="1:4">
+      <c r="A64" t="s">
+        <v>57</v>
+      </c>
+      <c r="B64">
+        <v>109</v>
+      </c>
+      <c r="C64">
+        <v>121</v>
+      </c>
+      <c r="D64" t="str">
         <f t="shared" si="0"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A58" t="s">
-        <v>30</v>
-      </c>
-      <c r="B58">
-        <v>133.5</v>
-      </c>
-      <c r="C58">
-        <v>146</v>
-      </c>
-      <c r="D58" t="str">
-        <f t="shared" si="0"/>
+    <row r="65" spans="1:4">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65">
+        <v>49</v>
+      </c>
+      <c r="C65">
+        <v>54.5</v>
+      </c>
+      <c r="D65" t="str">
+        <f t="shared" ref="D65:D67" si="1">IF(B65&lt;C65,"OT","ERC")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>35</v>
-      </c>
-      <c r="B59">
-        <v>63</v>
-      </c>
-      <c r="C59">
-        <v>67.5</v>
-      </c>
-      <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A60" t="s">
-        <v>38</v>
-      </c>
-      <c r="B60">
+    <row r="66" spans="1:4">
+      <c r="A66" t="s">
         <v>62</v>
       </c>
-      <c r="C60">
-        <v>68</v>
-      </c>
-      <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A61" t="s">
-        <v>39</v>
-      </c>
-      <c r="B61">
-        <v>62.5</v>
-      </c>
-      <c r="C61">
-        <v>63</v>
-      </c>
-      <c r="D61" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A62" t="s">
-        <v>42</v>
-      </c>
-      <c r="B62">
-        <v>145</v>
-      </c>
-      <c r="C62">
-        <v>155</v>
-      </c>
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A63" t="s">
-        <v>46</v>
-      </c>
-      <c r="B63">
-        <v>89</v>
-      </c>
-      <c r="C63">
-        <v>102</v>
-      </c>
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A64" t="s">
-        <v>52</v>
-      </c>
-      <c r="B64">
-        <v>142.5</v>
-      </c>
-      <c r="C64">
-        <v>151.5</v>
-      </c>
-      <c r="D64" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>55</v>
-      </c>
-      <c r="B65">
-        <v>75</v>
-      </c>
-      <c r="C65">
-        <v>79</v>
-      </c>
-      <c r="D65" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A66" t="s">
-        <v>59</v>
-      </c>
       <c r="B66">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C66">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A67" t="s">
-        <v>60</v>
-      </c>
-      <c r="B67">
-        <v>49</v>
-      </c>
-      <c r="C67">
-        <v>54.5</v>
-      </c>
-      <c r="D67" t="str">
-        <f t="shared" ref="D67:D69" si="1">IF(B67&lt;C67,"OT","ERC")</f>
-        <v>OT</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A68" t="s">
-        <v>64</v>
-      </c>
-      <c r="B68">
-        <v>100</v>
-      </c>
-      <c r="C68">
-        <v>104</v>
-      </c>
-      <c r="D68" t="str">
         <f t="shared" si="1"/>
         <v>OT</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A69" t="s">
-        <v>65</v>
-      </c>
-      <c r="B69">
+    <row r="67" spans="1:4">
+      <c r="A67" t="s">
+        <v>63</v>
+      </c>
+      <c r="B67">
         <v>140.5</v>
       </c>
-      <c r="C69">
+      <c r="C67">
         <v>190</v>
       </c>
-      <c r="D69" t="str">
+      <c r="D67" t="str">
         <f t="shared" si="1"/>
         <v>OT</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{EFB3B29F-8460-485E-9A7A-D16A554F19F3}">
-    <sortState ref="A2:D69">
+    <sortState ref="A2:D67">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5784AB59-AFE3-4BBC-A667-7392851A2225}">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" t="s">
-        <v>77</v>
-      </c>
       <c r="C1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>21</v>
+        <v>1279</v>
       </c>
       <c r="C2">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="D2">
-        <f>ABS(B2-C2)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" ref="D2:D45" si="0">ABS(B2-C2)</f>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1279</v>
+        <v>160</v>
       </c>
       <c r="C3">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D46" si="0">ABS(B3-C3)</f>
-        <v>1134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>241</v>
+      </c>
+      <c r="C4">
+        <v>153</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>160</v>
-      </c>
-      <c r="C4">
-        <v>158</v>
-      </c>
-      <c r="D4">
+      <c r="B5">
+        <v>189.5</v>
+      </c>
+      <c r="C5">
+        <v>187.5</v>
+      </c>
+      <c r="D5">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5">
-        <v>241</v>
-      </c>
-      <c r="C5">
-        <v>153</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
-        <v>88</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
-        <v>189.5</v>
+        <v>141</v>
       </c>
       <c r="C6">
-        <v>187.5</v>
+        <v>133.5</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>97</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B7">
-        <v>141</v>
-      </c>
-      <c r="C7">
-        <v>133.5</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>131</v>
+      </c>
+      <c r="C8">
+        <v>89</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
-        <v>105</v>
-      </c>
-      <c r="C8">
-        <v>97</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
       <c r="B9">
-        <v>131</v>
+        <v>57</v>
       </c>
       <c r="C9">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11">
-        <v>20</v>
+        <v>3500</v>
       </c>
       <c r="C11">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+        <v>3371</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12">
-        <v>3500</v>
+        <v>53</v>
       </c>
       <c r="C12">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>3371</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>146.5</v>
+      </c>
+      <c r="C13">
+        <v>90.5</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>53</v>
-      </c>
-      <c r="C13">
-        <v>51</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+      <c r="B14">
+        <v>19</v>
+      </c>
+      <c r="C14">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>146.5</v>
-      </c>
-      <c r="C14">
-        <v>90.5</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="B15">
+        <v>170</v>
+      </c>
+      <c r="C15">
+        <v>107</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
+      <c r="B16">
+        <v>5478</v>
+      </c>
+      <c r="C16">
+        <v>159</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>5319</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="C15">
-        <v>19</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16">
-        <v>170</v>
-      </c>
-      <c r="C16">
-        <v>107</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>20</v>
-      </c>
       <c r="B17">
-        <v>5478</v>
+        <v>5348.5</v>
       </c>
       <c r="C17">
-        <v>159</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>5319</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5309.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>21</v>
       </c>
       <c r="B18">
-        <v>5348.5</v>
+        <v>93</v>
       </c>
       <c r="C18">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>5309.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>93</v>
+        <v>16.5</v>
       </c>
       <c r="C19">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>24</v>
       </c>
       <c r="B20">
-        <v>16.5</v>
+        <v>954</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>189.5</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+        <v>764.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>26</v>
       </c>
       <c r="B21">
-        <v>954</v>
+        <v>3061</v>
       </c>
       <c r="C21">
-        <v>189.5</v>
+        <v>106.5</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>764.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2954.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>3061</v>
+        <v>132</v>
       </c>
       <c r="C22">
-        <v>106.5</v>
+        <v>129</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>2954.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>132</v>
+        <v>5426</v>
       </c>
       <c r="C23">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+        <v>5326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>5426</v>
+        <v>1729</v>
       </c>
       <c r="C24">
-        <v>100</v>
+        <v>148</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>5326</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+        <v>1581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>1729</v>
+        <v>2915</v>
       </c>
       <c r="C25">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>1581</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>2915</v>
+        <v>451.5</v>
       </c>
       <c r="C26">
-        <v>157</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>2758</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+        <v>408.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>451.5</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>43</v>
+        <v>49.5</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>408.5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>41</v>
       </c>
       <c r="B28">
-        <v>50</v>
+        <v>9723</v>
       </c>
       <c r="C28">
-        <v>49.5</v>
+        <v>44</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
+        <v>9679</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>97.5</v>
+      </c>
+      <c r="C29">
+        <v>97</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
-        <v>9723</v>
-      </c>
-      <c r="C29">
-        <v>44</v>
-      </c>
-      <c r="D29">
-        <f t="shared" si="0"/>
-        <v>9679</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>44</v>
-      </c>
       <c r="B30">
-        <v>97.5</v>
+        <v>90</v>
       </c>
       <c r="C30">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>45</v>
       </c>
       <c r="B31">
-        <v>90</v>
+        <v>248</v>
       </c>
       <c r="C31">
-        <v>86</v>
+        <v>229.5</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+        <v>18.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>2963</v>
+      </c>
+      <c r="C32">
+        <v>103</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>2860</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>47</v>
       </c>
-      <c r="B32">
-        <v>248</v>
-      </c>
-      <c r="C32">
-        <v>229.5</v>
-      </c>
-      <c r="D32">
-        <f t="shared" si="0"/>
-        <v>18.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
+      <c r="B33">
+        <v>96</v>
+      </c>
+      <c r="C33">
+        <v>91</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>48</v>
       </c>
-      <c r="B33">
-        <v>2963</v>
-      </c>
-      <c r="C33">
-        <v>103</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="0"/>
-        <v>2860</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
+      <c r="B34">
+        <v>51.5</v>
+      </c>
+      <c r="C34">
         <v>49</v>
       </c>
-      <c r="B34">
-        <v>96</v>
-      </c>
-      <c r="C34">
-        <v>91</v>
-      </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>51.5</v>
+        <v>274</v>
       </c>
       <c r="C35">
-        <v>49</v>
+        <v>104.5</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+        <v>169.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>51</v>
       </c>
       <c r="B36">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C36">
-        <v>104.5</v>
+        <v>88</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>169.5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B37">
-        <v>280</v>
+        <v>231</v>
       </c>
       <c r="C37">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" t="s">
         <v>54</v>
       </c>
       <c r="B38">
-        <v>231</v>
+        <v>184</v>
       </c>
       <c r="C38">
-        <v>105</v>
+        <v>168</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>232</v>
+      </c>
+      <c r="C39">
+        <v>221.5</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
         <v>56</v>
       </c>
-      <c r="B39">
-        <v>184</v>
-      </c>
-      <c r="C39">
-        <v>168</v>
-      </c>
-      <c r="D39">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>57</v>
-      </c>
       <c r="B40">
-        <v>232</v>
+        <v>19</v>
       </c>
       <c r="C40">
-        <v>221.5</v>
+        <v>19</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>10.5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B41">
-        <v>19</v>
+        <v>223</v>
       </c>
       <c r="C41">
-        <v>19</v>
+        <v>214</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" t="s">
+        <v>60</v>
+      </c>
+      <c r="B42">
+        <v>141</v>
+      </c>
+      <c r="C42">
+        <v>129</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" t="s">
         <v>61</v>
       </c>
-      <c r="B42">
-        <v>223</v>
-      </c>
-      <c r="C42">
-        <v>214</v>
-      </c>
-      <c r="D42">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>62</v>
-      </c>
       <c r="B43">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C43">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B44">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C44">
-        <v>100</v>
+        <v>118.5</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B45">
-        <v>119</v>
+        <v>414</v>
       </c>
       <c r="C45">
-        <v>118.5</v>
+        <v>147</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>67</v>
-      </c>
-      <c r="B46">
-        <v>414</v>
-      </c>
-      <c r="C46">
-        <v>147</v>
-      </c>
-      <c r="D46">
-        <f t="shared" si="0"/>
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A47" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1">
-        <f>AVERAGE($D$2:$D$46)</f>
-        <v>946.76666666666665</v>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="1"/>
+      <c r="C46" s="1"/>
+      <c r="D46" s="1">
+        <f>AVERAGE($D$2:$D$45)</f>
+        <v>968.23863636363637</v>
       </c>
     </row>
   </sheetData>
@@ -3001,337 +2950,322 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF24D01-91C4-401F-8722-EA056751A0DD}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
+        <v>147</v>
+      </c>
+      <c r="C2">
+        <v>159</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D20" si="0">ABS(B2-C2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
         <v>82.5</v>
       </c>
-      <c r="C2">
-        <v>86</v>
-      </c>
-      <c r="D2">
-        <f>ABS(B2-C2)</f>
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>147</v>
-      </c>
       <c r="C3">
-        <v>159</v>
+        <v>84</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D21" si="0">ABS(B3-C3)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B4">
-        <v>82.5</v>
+        <v>187</v>
       </c>
       <c r="C4">
-        <v>84</v>
+        <v>198.5</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>187</v>
+        <v>130</v>
       </c>
       <c r="C5">
-        <v>198.5</v>
+        <v>180</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>11.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6">
-        <v>130</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>180</v>
+        <v>52</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>25</v>
       </c>
       <c r="B7">
-        <v>50</v>
+        <v>177</v>
       </c>
       <c r="C7">
-        <v>52</v>
+        <v>184</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>27</v>
       </c>
       <c r="B8">
-        <v>177</v>
+        <v>115</v>
       </c>
       <c r="C8">
-        <v>184</v>
+        <v>122</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B9">
-        <v>115</v>
+        <v>133.5</v>
       </c>
       <c r="C9">
-        <v>122</v>
+        <v>146</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B10">
-        <v>133.5</v>
+        <v>63</v>
       </c>
       <c r="C10">
-        <v>146</v>
+        <v>67.5</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>12.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>68</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12">
+        <v>62.5</v>
+      </c>
+      <c r="C12">
         <v>63</v>
       </c>
-      <c r="C11">
-        <v>67.5</v>
-      </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13">
+        <v>145</v>
+      </c>
+      <c r="C13">
+        <v>155</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>89</v>
+      </c>
+      <c r="C14">
+        <v>102</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <v>142.5</v>
+      </c>
+      <c r="C15">
+        <v>151.5</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B16">
+        <v>75</v>
+      </c>
+      <c r="C16">
+        <v>79</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>109</v>
+      </c>
+      <c r="C17">
+        <v>121</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18">
+        <v>49</v>
+      </c>
+      <c r="C18">
+        <v>54.5</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>62</v>
       </c>
-      <c r="C12">
-        <v>68</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>39</v>
-      </c>
-      <c r="B13">
-        <v>62.5</v>
-      </c>
-      <c r="C13">
+      <c r="B19">
+        <v>100</v>
+      </c>
+      <c r="C19">
+        <v>104</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>63</v>
       </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>42</v>
-      </c>
-      <c r="B14">
-        <v>145</v>
-      </c>
-      <c r="C14">
-        <v>155</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B15">
-        <v>89</v>
-      </c>
-      <c r="C15">
-        <v>102</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>142.5</v>
-      </c>
-      <c r="C16">
-        <v>151.5</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17">
-        <v>75</v>
-      </c>
-      <c r="C17">
-        <v>79</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18">
-        <v>109</v>
-      </c>
-      <c r="C18">
-        <v>121</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19">
-        <v>49</v>
-      </c>
-      <c r="C19">
-        <v>54.5</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>64</v>
-      </c>
       <c r="B20">
-        <v>100</v>
+        <v>140.5</v>
       </c>
       <c r="C20">
-        <v>104</v>
+        <v>190</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>65</v>
-      </c>
-      <c r="B21">
-        <v>140.5</v>
-      </c>
-      <c r="C21">
-        <v>190</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="0"/>
         <v>49.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1">
-        <f>AVERAGE($D$2:$D$21)</f>
-        <v>11.25</v>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1">
+        <f>AVERAGE($D$2:$D$20)</f>
+        <v>11.657894736842104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
re-label Lang 67 and Lang 68 as Lang 01 and Lang 02
</commit_message>
<xml_diff>
--- a/results/compare_num_of_changes.xlsx
+++ b/results/compare_num_of_changes.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\linguist\Jou\projects\2021_RIP\Generals02\code\economy_RIPGLA\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\linguist\Jou\projects\2021_RIP\Generals02\code\Economy_RIPGLA-master\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD74FB46-EDDA-4593-9FDD-8C58D6CBBAA7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5185BC2D-CA06-40F4-AB1F-3D078158D29D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
   <si>
     <t>hypo03</t>
   </si>
@@ -270,6 +270,14 @@
   </si>
   <si>
     <t>N/A</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hypo01</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>hypo02</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1227,8 +1235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1879,7 +1887,7 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B44">
         <v>119</v>
@@ -1894,7 +1902,7 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B45">
         <v>414</v>

</xml_diff>

<commit_message>
Excluded Lang 14, 19, 59 from the list of languages more efficient under the ERC because they're ties
</commit_message>
<xml_diff>
--- a/results/compare_num_of_changes.xlsx
+++ b/results/compare_num_of_changes.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\linguist\Jou\projects\2021_RIP\Generals02\code\Economy_RIPGLA-master\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0699BCE5-13D5-456C-9C2D-4C5F0777062E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DC177-7949-4D24-BD34-40726B076790}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4155" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nonnoisy_changeinfo_original" sheetId="1" r:id="rId1"/>
-    <sheet name="OT_wins" sheetId="2" r:id="rId2"/>
-    <sheet name="ERC_wins" sheetId="3" r:id="rId3"/>
+    <sheet name="ERC_lower_median" sheetId="2" r:id="rId2"/>
+    <sheet name="OT_lower_median" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonnoisy_changeinfo_original!$A$1:$D$1</definedName>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
   <si>
     <t>hypo03</t>
   </si>
@@ -2258,10 +2258,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5784AB59-AFE3-4BBC-A667-7392851A2225}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -2321,7 +2321,7 @@
         <v>145</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D45" si="0">ABS(B4-C4)</f>
+        <f t="shared" ref="D4:D42" si="0">ABS(B4-C4)</f>
         <v>1134</v>
       </c>
     </row>
@@ -2432,268 +2432,268 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>3500</v>
       </c>
       <c r="C12">
-        <v>20</v>
+        <v>129</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3371</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B13">
-        <v>3500</v>
+        <v>53</v>
       </c>
       <c r="C13">
-        <v>129</v>
+        <v>51</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>3371</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14">
-        <v>53</v>
+        <v>146.5</v>
       </c>
       <c r="C14">
-        <v>51</v>
+        <v>90.5</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B15">
-        <v>146.5</v>
+        <v>170</v>
       </c>
       <c r="C15">
-        <v>90.5</v>
+        <v>107</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>56</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B16">
-        <v>19</v>
+        <v>5478</v>
       </c>
       <c r="C16">
-        <v>19</v>
+        <v>159</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5319</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B17">
-        <v>170</v>
+        <v>5348.5</v>
       </c>
       <c r="C17">
-        <v>107</v>
+        <v>39</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>63</v>
+        <v>5309.5</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B18">
-        <v>5478</v>
+        <v>93</v>
       </c>
       <c r="C18">
-        <v>159</v>
+        <v>83</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>5319</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B19">
-        <v>5348.5</v>
+        <v>16.5</v>
       </c>
       <c r="C19">
-        <v>39</v>
+        <v>16</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>5309.5</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B20">
-        <v>93</v>
+        <v>954</v>
       </c>
       <c r="C20">
-        <v>83</v>
+        <v>189.5</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>764.5</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B21">
-        <v>16.5</v>
+        <v>3061</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>106.5</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>2954.5</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B22">
-        <v>954</v>
+        <v>132</v>
       </c>
       <c r="C22">
-        <v>189.5</v>
+        <v>129</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>764.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B23">
-        <v>3061</v>
+        <v>5426</v>
       </c>
       <c r="C23">
-        <v>106.5</v>
+        <v>100</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>2954.5</v>
+        <v>5326</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B24">
-        <v>132</v>
+        <v>1729</v>
       </c>
       <c r="C24">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="B25">
-        <v>5426</v>
+        <v>2915</v>
       </c>
       <c r="C25">
-        <v>100</v>
+        <v>157</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>5326</v>
+        <v>2758</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B26">
-        <v>1729</v>
+        <v>451.5</v>
       </c>
       <c r="C26">
-        <v>148</v>
+        <v>43</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>1581</v>
+        <v>408.5</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B27">
-        <v>2915</v>
+        <v>50</v>
       </c>
       <c r="C27">
-        <v>157</v>
+        <v>49.5</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>2758</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B28">
-        <v>451.5</v>
+        <v>9723</v>
       </c>
       <c r="C28">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>408.5</v>
+        <v>9679</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B29">
-        <v>50</v>
+        <v>97.5</v>
       </c>
       <c r="C29">
-        <v>49.5</v>
+        <v>97</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
@@ -2702,259 +2702,214 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B30">
-        <v>9723</v>
+        <v>90</v>
       </c>
       <c r="C30">
-        <v>44</v>
+        <v>86</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>9679</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31">
-        <v>97.5</v>
+        <v>248</v>
       </c>
       <c r="C31">
-        <v>97</v>
+        <v>229.5</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B32">
-        <v>90</v>
+        <v>2963</v>
       </c>
       <c r="C32">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B33">
-        <v>248</v>
+        <v>96</v>
       </c>
       <c r="C33">
-        <v>229.5</v>
+        <v>91</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>18.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B34">
-        <v>2963</v>
+        <v>51.5</v>
       </c>
       <c r="C34">
-        <v>103</v>
+        <v>49</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>2860</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B35">
-        <v>96</v>
+        <v>274</v>
       </c>
       <c r="C35">
-        <v>91</v>
+        <v>104.5</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>169.5</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B36">
-        <v>51.5</v>
+        <v>280</v>
       </c>
       <c r="C36">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B37">
-        <v>274</v>
+        <v>231</v>
       </c>
       <c r="C37">
-        <v>104.5</v>
+        <v>105</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>169.5</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B38">
-        <v>280</v>
+        <v>184</v>
       </c>
       <c r="C38">
-        <v>88</v>
+        <v>168</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>16</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B39">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C39">
-        <v>105</v>
+        <v>221.5</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>126</v>
+        <v>10.5</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B40">
-        <v>184</v>
+        <v>223</v>
       </c>
       <c r="C40">
-        <v>168</v>
+        <v>214</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B41">
-        <v>232</v>
+        <v>141</v>
       </c>
       <c r="C41">
-        <v>221.5</v>
+        <v>129</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>10.5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B42">
-        <v>19</v>
+        <v>117</v>
       </c>
       <c r="C42">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43">
-        <v>223</v>
-      </c>
-      <c r="C43">
-        <v>214</v>
-      </c>
-      <c r="D43">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44">
-        <v>141</v>
-      </c>
-      <c r="C44">
-        <v>129</v>
-      </c>
-      <c r="D44">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45">
-        <v>117</v>
-      </c>
-      <c r="C45">
-        <v>100</v>
-      </c>
-      <c r="D45">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="1" t="s">
+      <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1">
-        <f>AVERAGE($D$4:$D$45)</f>
-        <v>1007.9761904761905</v>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1">
+        <f>AVERAGE(D2:D42)</f>
+        <v>1039.0853658536585</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2962,8 +2917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF24D01-91C4-401F-8722-EA056751A0DD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -3274,7 +3229,7 @@
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1">
-        <f>AVERAGE($D$2:$D$20)</f>
+        <f>AVERAGE(D2:D20)</f>
         <v>11.657894736842104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revised function for determining ERC vs. OT win in # of grammar changes, to accurately account for ties
</commit_message>
<xml_diff>
--- a/results/compare_num_of_changes.xlsx
+++ b/results/compare_num_of_changes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\linguist\Jou\projects\2021_RIP\Generals02\code\Economy_RIPGLA-master\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{413DC177-7949-4D24-BD34-40726B076790}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDE8D3A-04D8-42AE-8685-CC50B6DEC922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="4155" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="nonnoisy_changeinfo_original" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,44 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">nonnoisy_changeinfo_original!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="80">
   <si>
     <t>hypo03</t>
   </si>
@@ -287,7 +320,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1237,13 +1270,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>64</v>
       </c>
@@ -1257,7 +1290,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>76</v>
       </c>
@@ -1267,12 +1300,12 @@
       <c r="C2">
         <v>118.5</v>
       </c>
-      <c r="D2" t="str">
-        <f>IF(B2&lt;C2,"OT","ERC")</f>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="D2" t="str" cm="1">
+        <f t="array" ref="D2">_xlfn.IFS(AND(B2&lt;C2, AND(NOT(ISTEXT(B2)), NOT(ISTEXT(C2)))),"OT", AND(B2&gt;C2, AND(NOT(ISTEXT(B2)), NOT(ISTEXT(C2)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>77</v>
       </c>
@@ -1282,12 +1315,12 @@
       <c r="C3">
         <v>147</v>
       </c>
-      <c r="D3" t="str">
-        <f>IF(B3&lt;C3,"OT","ERC")</f>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="D3" t="str" cm="1">
+        <f t="array" ref="D3">_xlfn.IFS(AND(B3&lt;C3, AND(NOT(ISTEXT(B3)), NOT(ISTEXT(C3)))),"OT", AND(B3&gt;C3, AND(NOT(ISTEXT(B3)), NOT(ISTEXT(C3)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1297,12 +1330,12 @@
       <c r="C4">
         <v>145</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D64" si="0">IF(B4&lt;C4,"OT","ERC")</f>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="D4" t="str" cm="1">
+        <f t="array" ref="D4">_xlfn.IFS(AND(B4&lt;C4, AND(NOT(ISTEXT(B4)), NOT(ISTEXT(C4)))),"OT", AND(B4&gt;C4, AND(NOT(ISTEXT(B4)), NOT(ISTEXT(C4)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1312,12 +1345,12 @@
       <c r="C5">
         <v>158</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="D5" t="str" cm="1">
+        <f t="array" ref="D5">_xlfn.IFS(AND(B5&lt;C5, AND(NOT(ISTEXT(B5)), NOT(ISTEXT(C5)))),"OT", AND(B5&gt;C5, AND(NOT(ISTEXT(B5)), NOT(ISTEXT(C5)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1327,12 +1360,12 @@
       <c r="C6">
         <v>153</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="D6" t="str" cm="1">
+        <f t="array" ref="D6">_xlfn.IFS(AND(B6&lt;C6, AND(NOT(ISTEXT(B6)), NOT(ISTEXT(C6)))),"OT", AND(B6&gt;C6, AND(NOT(ISTEXT(B6)), NOT(ISTEXT(C6)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1342,12 +1375,12 @@
       <c r="C7">
         <v>187.5</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="D7" t="str" cm="1">
+        <f t="array" ref="D7">_xlfn.IFS(AND(B7&lt;C7, AND(NOT(ISTEXT(B7)), NOT(ISTEXT(C7)))),"OT", AND(B7&gt;C7, AND(NOT(ISTEXT(B7)), NOT(ISTEXT(C7)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1357,12 +1390,12 @@
       <c r="C8">
         <v>133.5</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="D8" t="str" cm="1">
+        <f t="array" ref="D8">_xlfn.IFS(AND(B8&lt;C8, AND(NOT(ISTEXT(B8)), NOT(ISTEXT(C8)))),"OT", AND(B8&gt;C8, AND(NOT(ISTEXT(B8)), NOT(ISTEXT(C8)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1372,12 +1405,12 @@
       <c r="C9">
         <v>97</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="D9" t="str" cm="1">
+        <f t="array" ref="D9">_xlfn.IFS(AND(B9&lt;C9, AND(NOT(ISTEXT(B9)), NOT(ISTEXT(C9)))),"OT", AND(B9&gt;C9, AND(NOT(ISTEXT(B9)), NOT(ISTEXT(C9)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1387,12 +1420,12 @@
       <c r="C10">
         <v>89</v>
       </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="D10" t="str" cm="1">
+        <f t="array" ref="D10">_xlfn.IFS(AND(B10&lt;C10, AND(NOT(ISTEXT(B10)), NOT(ISTEXT(C10)))),"OT", AND(B10&gt;C10, AND(NOT(ISTEXT(B10)), NOT(ISTEXT(C10)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1402,522 +1435,522 @@
       <c r="C11">
         <v>54</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="D11" t="str" cm="1">
+        <f t="array" ref="D11">_xlfn.IFS(AND(B11&lt;C11, AND(NOT(ISTEXT(B11)), NOT(ISTEXT(C11)))),"OT", AND(B11&gt;C11, AND(NOT(ISTEXT(B11)), NOT(ISTEXT(C11)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>3500</v>
+      </c>
+      <c r="C12">
+        <v>129</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" ref="D12">_xlfn.IFS(AND(B12&lt;C12, AND(NOT(ISTEXT(B12)), NOT(ISTEXT(C12)))),"OT", AND(B12&gt;C12, AND(NOT(ISTEXT(B12)), NOT(ISTEXT(C12)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>53</v>
+      </c>
+      <c r="C13">
+        <v>51</v>
+      </c>
+      <c r="D13" t="str" cm="1">
+        <f t="array" ref="D13">_xlfn.IFS(AND(B13&lt;C13, AND(NOT(ISTEXT(B13)), NOT(ISTEXT(C13)))),"OT", AND(B13&gt;C13, AND(NOT(ISTEXT(B13)), NOT(ISTEXT(C13)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>146.5</v>
+      </c>
+      <c r="C14">
+        <v>90.5</v>
+      </c>
+      <c r="D14" t="str" cm="1">
+        <f t="array" ref="D14">_xlfn.IFS(AND(B14&lt;C14, AND(NOT(ISTEXT(B14)), NOT(ISTEXT(C14)))),"OT", AND(B14&gt;C14, AND(NOT(ISTEXT(B14)), NOT(ISTEXT(C14)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>170</v>
+      </c>
+      <c r="C15">
+        <v>107</v>
+      </c>
+      <c r="D15" t="str" cm="1">
+        <f t="array" ref="D15">_xlfn.IFS(AND(B15&lt;C15, AND(NOT(ISTEXT(B15)), NOT(ISTEXT(C15)))),"OT", AND(B15&gt;C15, AND(NOT(ISTEXT(B15)), NOT(ISTEXT(C15)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>5478</v>
+      </c>
+      <c r="C16">
+        <v>159</v>
+      </c>
+      <c r="D16" t="str" cm="1">
+        <f t="array" ref="D16">_xlfn.IFS(AND(B16&lt;C16, AND(NOT(ISTEXT(B16)), NOT(ISTEXT(C16)))),"OT", AND(B16&gt;C16, AND(NOT(ISTEXT(B16)), NOT(ISTEXT(C16)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17">
+        <v>5348.5</v>
+      </c>
+      <c r="C17">
+        <v>39</v>
+      </c>
+      <c r="D17" t="str" cm="1">
+        <f t="array" ref="D17">_xlfn.IFS(AND(B17&lt;C17, AND(NOT(ISTEXT(B17)), NOT(ISTEXT(C17)))),"OT", AND(B17&gt;C17, AND(NOT(ISTEXT(B17)), NOT(ISTEXT(C17)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18">
+        <v>93</v>
+      </c>
+      <c r="C18">
+        <v>83</v>
+      </c>
+      <c r="D18" t="str" cm="1">
+        <f t="array" ref="D18">_xlfn.IFS(AND(B18&lt;C18, AND(NOT(ISTEXT(B18)), NOT(ISTEXT(C18)))),"OT", AND(B18&gt;C18, AND(NOT(ISTEXT(B18)), NOT(ISTEXT(C18)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>16.5</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" t="str" cm="1">
+        <f t="array" ref="D19">_xlfn.IFS(AND(B19&lt;C19, AND(NOT(ISTEXT(B19)), NOT(ISTEXT(C19)))),"OT", AND(B19&gt;C19, AND(NOT(ISTEXT(B19)), NOT(ISTEXT(C19)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>954</v>
+      </c>
+      <c r="C20">
+        <v>189.5</v>
+      </c>
+      <c r="D20" t="str" cm="1">
+        <f t="array" ref="D20">_xlfn.IFS(AND(B20&lt;C20, AND(NOT(ISTEXT(B20)), NOT(ISTEXT(C20)))),"OT", AND(B20&gt;C20, AND(NOT(ISTEXT(B20)), NOT(ISTEXT(C20)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>3061</v>
+      </c>
+      <c r="C21">
+        <v>106.5</v>
+      </c>
+      <c r="D21" t="str" cm="1">
+        <f t="array" ref="D21">_xlfn.IFS(AND(B21&lt;C21, AND(NOT(ISTEXT(B21)), NOT(ISTEXT(C21)))),"OT", AND(B21&gt;C21, AND(NOT(ISTEXT(B21)), NOT(ISTEXT(C21)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>132</v>
+      </c>
+      <c r="C22">
+        <v>129</v>
+      </c>
+      <c r="D22" t="str" cm="1">
+        <f t="array" ref="D22">_xlfn.IFS(AND(B22&lt;C22, AND(NOT(ISTEXT(B22)), NOT(ISTEXT(C22)))),"OT", AND(B22&gt;C22, AND(NOT(ISTEXT(B22)), NOT(ISTEXT(C22)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>5426</v>
+      </c>
+      <c r="C23">
+        <v>100</v>
+      </c>
+      <c r="D23" t="str" cm="1">
+        <f t="array" ref="D23">_xlfn.IFS(AND(B23&lt;C23, AND(NOT(ISTEXT(B23)), NOT(ISTEXT(C23)))),"OT", AND(B23&gt;C23, AND(NOT(ISTEXT(B23)), NOT(ISTEXT(C23)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24">
+        <v>1729</v>
+      </c>
+      <c r="C24">
+        <v>148</v>
+      </c>
+      <c r="D24" t="str" cm="1">
+        <f t="array" ref="D24">_xlfn.IFS(AND(B24&lt;C24, AND(NOT(ISTEXT(B24)), NOT(ISTEXT(C24)))),"OT", AND(B24&gt;C24, AND(NOT(ISTEXT(B24)), NOT(ISTEXT(C24)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25">
+        <v>2915</v>
+      </c>
+      <c r="C25">
+        <v>157</v>
+      </c>
+      <c r="D25" t="str" cm="1">
+        <f t="array" ref="D25">_xlfn.IFS(AND(B25&lt;C25, AND(NOT(ISTEXT(B25)), NOT(ISTEXT(C25)))),"OT", AND(B25&gt;C25, AND(NOT(ISTEXT(B25)), NOT(ISTEXT(C25)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+      <c r="B26">
+        <v>451.5</v>
+      </c>
+      <c r="C26">
+        <v>43</v>
+      </c>
+      <c r="D26" t="str" cm="1">
+        <f t="array" ref="D26">_xlfn.IFS(AND(B26&lt;C26, AND(NOT(ISTEXT(B26)), NOT(ISTEXT(C26)))),"OT", AND(B26&gt;C26, AND(NOT(ISTEXT(B26)), NOT(ISTEXT(C26)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27">
+        <v>50</v>
+      </c>
+      <c r="C27">
+        <v>49.5</v>
+      </c>
+      <c r="D27" t="str" cm="1">
+        <f t="array" ref="D27">_xlfn.IFS(AND(B27&lt;C27, AND(NOT(ISTEXT(B27)), NOT(ISTEXT(C27)))),"OT", AND(B27&gt;C27, AND(NOT(ISTEXT(B27)), NOT(ISTEXT(C27)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28">
+        <v>9723</v>
+      </c>
+      <c r="C28">
+        <v>44</v>
+      </c>
+      <c r="D28" t="str" cm="1">
+        <f t="array" ref="D28">_xlfn.IFS(AND(B28&lt;C28, AND(NOT(ISTEXT(B28)), NOT(ISTEXT(C28)))),"OT", AND(B28&gt;C28, AND(NOT(ISTEXT(B28)), NOT(ISTEXT(C28)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29">
+        <v>97.5</v>
+      </c>
+      <c r="C29">
+        <v>97</v>
+      </c>
+      <c r="D29" t="str" cm="1">
+        <f t="array" ref="D29">_xlfn.IFS(AND(B29&lt;C29, AND(NOT(ISTEXT(B29)), NOT(ISTEXT(C29)))),"OT", AND(B29&gt;C29, AND(NOT(ISTEXT(B29)), NOT(ISTEXT(C29)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30">
+        <v>90</v>
+      </c>
+      <c r="C30">
+        <v>86</v>
+      </c>
+      <c r="D30" t="str" cm="1">
+        <f t="array" ref="D30">_xlfn.IFS(AND(B30&lt;C30, AND(NOT(ISTEXT(B30)), NOT(ISTEXT(C30)))),"OT", AND(B30&gt;C30, AND(NOT(ISTEXT(B30)), NOT(ISTEXT(C30)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31">
+        <v>248</v>
+      </c>
+      <c r="C31">
+        <v>229.5</v>
+      </c>
+      <c r="D31" t="str" cm="1">
+        <f t="array" ref="D31">_xlfn.IFS(AND(B31&lt;C31, AND(NOT(ISTEXT(B31)), NOT(ISTEXT(C31)))),"OT", AND(B31&gt;C31, AND(NOT(ISTEXT(B31)), NOT(ISTEXT(C31)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32">
+        <v>2963</v>
+      </c>
+      <c r="C32">
+        <v>103</v>
+      </c>
+      <c r="D32" t="str" cm="1">
+        <f t="array" ref="D32">_xlfn.IFS(AND(B32&lt;C32, AND(NOT(ISTEXT(B32)), NOT(ISTEXT(C32)))),"OT", AND(B32&gt;C32, AND(NOT(ISTEXT(B32)), NOT(ISTEXT(C32)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33">
+        <v>96</v>
+      </c>
+      <c r="C33">
+        <v>91</v>
+      </c>
+      <c r="D33" t="str" cm="1">
+        <f t="array" ref="D33">_xlfn.IFS(AND(B33&lt;C33, AND(NOT(ISTEXT(B33)), NOT(ISTEXT(C33)))),"OT", AND(B33&gt;C33, AND(NOT(ISTEXT(B33)), NOT(ISTEXT(C33)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34">
+        <v>51.5</v>
+      </c>
+      <c r="C34">
+        <v>49</v>
+      </c>
+      <c r="D34" t="str" cm="1">
+        <f t="array" ref="D34">_xlfn.IFS(AND(B34&lt;C34, AND(NOT(ISTEXT(B34)), NOT(ISTEXT(C34)))),"OT", AND(B34&gt;C34, AND(NOT(ISTEXT(B34)), NOT(ISTEXT(C34)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35">
+        <v>274</v>
+      </c>
+      <c r="C35">
+        <v>104.5</v>
+      </c>
+      <c r="D35" t="str" cm="1">
+        <f t="array" ref="D35">_xlfn.IFS(AND(B35&lt;C35, AND(NOT(ISTEXT(B35)), NOT(ISTEXT(C35)))),"OT", AND(B35&gt;C35, AND(NOT(ISTEXT(B35)), NOT(ISTEXT(C35)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36">
+        <v>280</v>
+      </c>
+      <c r="C36">
+        <v>88</v>
+      </c>
+      <c r="D36" t="str" cm="1">
+        <f t="array" ref="D36">_xlfn.IFS(AND(B36&lt;C36, AND(NOT(ISTEXT(B36)), NOT(ISTEXT(C36)))),"OT", AND(B36&gt;C36, AND(NOT(ISTEXT(B36)), NOT(ISTEXT(C36)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37">
+        <v>231</v>
+      </c>
+      <c r="C37">
+        <v>105</v>
+      </c>
+      <c r="D37" t="str" cm="1">
+        <f t="array" ref="D37">_xlfn.IFS(AND(B37&lt;C37, AND(NOT(ISTEXT(B37)), NOT(ISTEXT(C37)))),"OT", AND(B37&gt;C37, AND(NOT(ISTEXT(B37)), NOT(ISTEXT(C37)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38">
+        <v>184</v>
+      </c>
+      <c r="C38">
+        <v>168</v>
+      </c>
+      <c r="D38" t="str" cm="1">
+        <f t="array" ref="D38">_xlfn.IFS(AND(B38&lt;C38, AND(NOT(ISTEXT(B38)), NOT(ISTEXT(C38)))),"OT", AND(B38&gt;C38, AND(NOT(ISTEXT(B38)), NOT(ISTEXT(C38)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
+        <v>55</v>
+      </c>
+      <c r="B39">
+        <v>232</v>
+      </c>
+      <c r="C39">
+        <v>221.5</v>
+      </c>
+      <c r="D39" t="str" cm="1">
+        <f t="array" ref="D39">_xlfn.IFS(AND(B39&lt;C39, AND(NOT(ISTEXT(B39)), NOT(ISTEXT(C39)))),"OT", AND(B39&gt;C39, AND(NOT(ISTEXT(B39)), NOT(ISTEXT(C39)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40">
+        <v>223</v>
+      </c>
+      <c r="C40">
+        <v>214</v>
+      </c>
+      <c r="D40" t="str" cm="1">
+        <f t="array" ref="D40">_xlfn.IFS(AND(B40&lt;C40, AND(NOT(ISTEXT(B40)), NOT(ISTEXT(C40)))),"OT", AND(B40&gt;C40, AND(NOT(ISTEXT(B40)), NOT(ISTEXT(C40)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41">
+        <v>141</v>
+      </c>
+      <c r="C41">
+        <v>129</v>
+      </c>
+      <c r="D41" t="str" cm="1">
+        <f t="array" ref="D41">_xlfn.IFS(AND(B41&lt;C41, AND(NOT(ISTEXT(B41)), NOT(ISTEXT(C41)))),"OT", AND(B41&gt;C41, AND(NOT(ISTEXT(B41)), NOT(ISTEXT(C41)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
+        <v>61</v>
+      </c>
+      <c r="B42">
+        <v>117</v>
+      </c>
+      <c r="C42">
+        <v>100</v>
+      </c>
+      <c r="D42" t="str" cm="1">
+        <f t="array" ref="D42">_xlfn.IFS(AND(B42&lt;C42, AND(NOT(ISTEXT(B42)), NOT(ISTEXT(C42)))),"OT", AND(B42&gt;C42, AND(NOT(ISTEXT(B42)), NOT(ISTEXT(C42)))), "ERC", TRUE, "N/A")</f>
+        <v>ERC</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
         <v>11</v>
       </c>
-      <c r="B12">
+      <c r="B43">
         <v>20</v>
       </c>
-      <c r="C12">
+      <c r="C43">
         <v>20</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>3500</v>
-      </c>
-      <c r="C13">
-        <v>129</v>
-      </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
-        <v>53</v>
-      </c>
-      <c r="C14">
-        <v>51</v>
-      </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15">
-        <v>146.5</v>
-      </c>
-      <c r="C15">
-        <v>90.5</v>
-      </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
-      <c r="A16" t="s">
+      <c r="D43" t="str" cm="1">
+        <f t="array" ref="D43">_xlfn.IFS(AND(B43&lt;C43, AND(NOT(ISTEXT(B43)), NOT(ISTEXT(C43)))),"OT", AND(B43&gt;C43, AND(NOT(ISTEXT(B43)), NOT(ISTEXT(C43)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B44">
         <v>19</v>
       </c>
-      <c r="C16">
+      <c r="C44">
         <v>19</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17">
-        <v>170</v>
-      </c>
-      <c r="C17">
-        <v>107</v>
-      </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18">
-        <v>5478</v>
-      </c>
-      <c r="C18">
-        <v>159</v>
-      </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
-      <c r="A19" t="s">
+      <c r="D44" t="str" cm="1">
+        <f t="array" ref="D44">_xlfn.IFS(AND(B44&lt;C44, AND(NOT(ISTEXT(B44)), NOT(ISTEXT(C44)))),"OT", AND(B44&gt;C44, AND(NOT(ISTEXT(B44)), NOT(ISTEXT(C44)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B45">
         <v>19</v>
       </c>
-      <c r="B19">
-        <v>5348.5</v>
-      </c>
-      <c r="C19">
-        <v>39</v>
-      </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20">
-        <v>93</v>
-      </c>
-      <c r="C20">
-        <v>83</v>
-      </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21">
-        <v>16.5</v>
-      </c>
-      <c r="C21">
-        <v>16</v>
-      </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22">
-        <v>954</v>
-      </c>
-      <c r="C22">
-        <v>189.5</v>
-      </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23">
-        <v>3061</v>
-      </c>
-      <c r="C23">
-        <v>106.5</v>
-      </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
-        <v>132</v>
-      </c>
-      <c r="C24">
-        <v>129</v>
-      </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
-        <v>5426</v>
-      </c>
-      <c r="C25">
-        <v>100</v>
-      </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" t="s">
-        <v>34</v>
-      </c>
-      <c r="B26">
-        <v>1729</v>
-      </c>
-      <c r="C26">
-        <v>148</v>
-      </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" t="s">
-        <v>35</v>
-      </c>
-      <c r="B27">
-        <v>2915</v>
-      </c>
-      <c r="C27">
-        <v>157</v>
-      </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B28">
-        <v>451.5</v>
-      </c>
-      <c r="C28">
-        <v>43</v>
-      </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" t="s">
-        <v>39</v>
-      </c>
-      <c r="B29">
-        <v>50</v>
-      </c>
-      <c r="C29">
-        <v>49.5</v>
-      </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" t="s">
-        <v>41</v>
-      </c>
-      <c r="B30">
-        <v>9723</v>
-      </c>
-      <c r="C30">
-        <v>44</v>
-      </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B31">
-        <v>97.5</v>
-      </c>
-      <c r="C31">
-        <v>97</v>
-      </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" t="s">
-        <v>43</v>
-      </c>
-      <c r="B32">
-        <v>90</v>
-      </c>
-      <c r="C32">
-        <v>86</v>
-      </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33">
-        <v>248</v>
-      </c>
-      <c r="C33">
-        <v>229.5</v>
-      </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34">
-        <v>2963</v>
-      </c>
-      <c r="C34">
-        <v>103</v>
-      </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35">
-        <v>96</v>
-      </c>
-      <c r="C35">
-        <v>91</v>
-      </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36">
-        <v>51.5</v>
-      </c>
-      <c r="C36">
-        <v>49</v>
-      </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" t="s">
-        <v>49</v>
-      </c>
-      <c r="B37">
-        <v>274</v>
-      </c>
-      <c r="C37">
-        <v>104.5</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" t="s">
-        <v>51</v>
-      </c>
-      <c r="B38">
-        <v>280</v>
-      </c>
-      <c r="C38">
-        <v>88</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B39">
-        <v>231</v>
-      </c>
-      <c r="C39">
-        <v>105</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40">
-        <v>184</v>
-      </c>
-      <c r="C40">
-        <v>168</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" t="s">
-        <v>55</v>
-      </c>
-      <c r="B41">
-        <v>232</v>
-      </c>
-      <c r="C41">
-        <v>221.5</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
-      <c r="A42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42">
+      <c r="C45">
         <v>19</v>
       </c>
-      <c r="C42">
-        <v>19</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43">
-        <v>223</v>
-      </c>
-      <c r="C43">
-        <v>214</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
-      <c r="A44" t="s">
-        <v>60</v>
-      </c>
-      <c r="B44">
-        <v>141</v>
-      </c>
-      <c r="C44">
-        <v>129</v>
-      </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
-      <c r="A45" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45">
-        <v>117</v>
-      </c>
-      <c r="C45">
-        <v>100</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>ERC</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+      <c r="D45" t="str" cm="1">
+        <f t="array" ref="D45">_xlfn.IFS(AND(B45&lt;C45, AND(NOT(ISTEXT(B45)), NOT(ISTEXT(C45)))),"OT", AND(B45&gt;C45, AND(NOT(ISTEXT(B45)), NOT(ISTEXT(C45)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>10</v>
       </c>
@@ -1927,11 +1960,12 @@
       <c r="C46">
         <v>91</v>
       </c>
-      <c r="D46" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+      <c r="D46" t="str" cm="1">
+        <f t="array" ref="D46">_xlfn.IFS(AND(B46&lt;C46, AND(NOT(ISTEXT(B46)), NOT(ISTEXT(C46)))),"OT", AND(B46&gt;C46, AND(NOT(ISTEXT(B46)), NOT(ISTEXT(C46)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>31</v>
       </c>
@@ -1941,11 +1975,12 @@
       <c r="C47" t="s">
         <v>75</v>
       </c>
-      <c r="D47" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+      <c r="D47" t="str" cm="1">
+        <f t="array" ref="D47">_xlfn.IFS(AND(B47&lt;C47, AND(NOT(ISTEXT(B47)), NOT(ISTEXT(C47)))),"OT", AND(B47&gt;C47, AND(NOT(ISTEXT(B47)), NOT(ISTEXT(C47)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>32</v>
       </c>
@@ -1955,11 +1990,12 @@
       <c r="C48" t="s">
         <v>75</v>
       </c>
-      <c r="D48" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+      <c r="D48" t="str" cm="1">
+        <f t="array" ref="D48">_xlfn.IFS(AND(B48&lt;C48, AND(NOT(ISTEXT(B48)), NOT(ISTEXT(C48)))),"OT", AND(B48&gt;C48, AND(NOT(ISTEXT(B48)), NOT(ISTEXT(C48)))), "ERC", TRUE, "N/A")</f>
+        <v>N/A</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>1</v>
       </c>
@@ -1969,12 +2005,12 @@
       <c r="C49">
         <v>159</v>
       </c>
-      <c r="D49" t="str">
-        <f t="shared" si="0"/>
+      <c r="D49" t="str" cm="1">
+        <f t="array" ref="D49">_xlfn.IFS(AND(B49&lt;C49, AND(NOT(ISTEXT(B49)), NOT(ISTEXT(C49)))),"OT", AND(B49&gt;C49, AND(NOT(ISTEXT(B49)), NOT(ISTEXT(C49)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>5</v>
       </c>
@@ -1984,12 +2020,12 @@
       <c r="C50">
         <v>84</v>
       </c>
-      <c r="D50" t="str">
-        <f t="shared" si="0"/>
+      <c r="D50" t="str" cm="1">
+        <f t="array" ref="D50">_xlfn.IFS(AND(B50&lt;C50, AND(NOT(ISTEXT(B50)), NOT(ISTEXT(C50)))),"OT", AND(B50&gt;C50, AND(NOT(ISTEXT(B50)), NOT(ISTEXT(C50)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>13</v>
       </c>
@@ -1999,12 +2035,12 @@
       <c r="C51">
         <v>198.5</v>
       </c>
-      <c r="D51" t="str">
-        <f t="shared" si="0"/>
+      <c r="D51" t="str" cm="1">
+        <f t="array" ref="D51">_xlfn.IFS(AND(B51&lt;C51, AND(NOT(ISTEXT(B51)), NOT(ISTEXT(C51)))),"OT", AND(B51&gt;C51, AND(NOT(ISTEXT(B51)), NOT(ISTEXT(C51)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>20</v>
       </c>
@@ -2014,12 +2050,12 @@
       <c r="C52">
         <v>180</v>
       </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
+      <c r="D52" t="str" cm="1">
+        <f t="array" ref="D52">_xlfn.IFS(AND(B52&lt;C52, AND(NOT(ISTEXT(B52)), NOT(ISTEXT(C52)))),"OT", AND(B52&gt;C52, AND(NOT(ISTEXT(B52)), NOT(ISTEXT(C52)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>23</v>
       </c>
@@ -2029,12 +2065,12 @@
       <c r="C53">
         <v>52</v>
       </c>
-      <c r="D53" t="str">
-        <f t="shared" si="0"/>
+      <c r="D53" t="str" cm="1">
+        <f t="array" ref="D53">_xlfn.IFS(AND(B53&lt;C53, AND(NOT(ISTEXT(B53)), NOT(ISTEXT(C53)))),"OT", AND(B53&gt;C53, AND(NOT(ISTEXT(B53)), NOT(ISTEXT(C53)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>25</v>
       </c>
@@ -2044,12 +2080,12 @@
       <c r="C54">
         <v>184</v>
       </c>
-      <c r="D54" t="str">
-        <f t="shared" si="0"/>
+      <c r="D54" t="str" cm="1">
+        <f t="array" ref="D54">_xlfn.IFS(AND(B54&lt;C54, AND(NOT(ISTEXT(B54)), NOT(ISTEXT(C54)))),"OT", AND(B54&gt;C54, AND(NOT(ISTEXT(B54)), NOT(ISTEXT(C54)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -2059,12 +2095,12 @@
       <c r="C55">
         <v>122</v>
       </c>
-      <c r="D55" t="str">
-        <f t="shared" si="0"/>
+      <c r="D55" t="str" cm="1">
+        <f t="array" ref="D55">_xlfn.IFS(AND(B55&lt;C55, AND(NOT(ISTEXT(B55)), NOT(ISTEXT(C55)))),"OT", AND(B55&gt;C55, AND(NOT(ISTEXT(B55)), NOT(ISTEXT(C55)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>28</v>
       </c>
@@ -2074,12 +2110,12 @@
       <c r="C56">
         <v>146</v>
       </c>
-      <c r="D56" t="str">
-        <f t="shared" si="0"/>
+      <c r="D56" t="str" cm="1">
+        <f t="array" ref="D56">_xlfn.IFS(AND(B56&lt;C56, AND(NOT(ISTEXT(B56)), NOT(ISTEXT(C56)))),"OT", AND(B56&gt;C56, AND(NOT(ISTEXT(B56)), NOT(ISTEXT(C56)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>33</v>
       </c>
@@ -2089,12 +2125,12 @@
       <c r="C57">
         <v>67.5</v>
       </c>
-      <c r="D57" t="str">
-        <f t="shared" si="0"/>
+      <c r="D57" t="str" cm="1">
+        <f t="array" ref="D57">_xlfn.IFS(AND(B57&lt;C57, AND(NOT(ISTEXT(B57)), NOT(ISTEXT(C57)))),"OT", AND(B57&gt;C57, AND(NOT(ISTEXT(B57)), NOT(ISTEXT(C57)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>36</v>
       </c>
@@ -2104,12 +2140,12 @@
       <c r="C58">
         <v>68</v>
       </c>
-      <c r="D58" t="str">
-        <f t="shared" si="0"/>
+      <c r="D58" t="str" cm="1">
+        <f t="array" ref="D58">_xlfn.IFS(AND(B58&lt;C58, AND(NOT(ISTEXT(B58)), NOT(ISTEXT(C58)))),"OT", AND(B58&gt;C58, AND(NOT(ISTEXT(B58)), NOT(ISTEXT(C58)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>37</v>
       </c>
@@ -2119,12 +2155,12 @@
       <c r="C59">
         <v>63</v>
       </c>
-      <c r="D59" t="str">
-        <f t="shared" si="0"/>
+      <c r="D59" t="str" cm="1">
+        <f t="array" ref="D59">_xlfn.IFS(AND(B59&lt;C59, AND(NOT(ISTEXT(B59)), NOT(ISTEXT(C59)))),"OT", AND(B59&gt;C59, AND(NOT(ISTEXT(B59)), NOT(ISTEXT(C59)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>40</v>
       </c>
@@ -2134,12 +2170,12 @@
       <c r="C60">
         <v>155</v>
       </c>
-      <c r="D60" t="str">
-        <f t="shared" si="0"/>
+      <c r="D60" t="str" cm="1">
+        <f t="array" ref="D60">_xlfn.IFS(AND(B60&lt;C60, AND(NOT(ISTEXT(B60)), NOT(ISTEXT(C60)))),"OT", AND(B60&gt;C60, AND(NOT(ISTEXT(B60)), NOT(ISTEXT(C60)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>44</v>
       </c>
@@ -2149,12 +2185,12 @@
       <c r="C61">
         <v>102</v>
       </c>
-      <c r="D61" t="str">
-        <f t="shared" si="0"/>
+      <c r="D61" t="str" cm="1">
+        <f t="array" ref="D61">_xlfn.IFS(AND(B61&lt;C61, AND(NOT(ISTEXT(B61)), NOT(ISTEXT(C61)))),"OT", AND(B61&gt;C61, AND(NOT(ISTEXT(B61)), NOT(ISTEXT(C61)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>50</v>
       </c>
@@ -2164,12 +2200,12 @@
       <c r="C62">
         <v>151.5</v>
       </c>
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
+      <c r="D62" t="str" cm="1">
+        <f t="array" ref="D62">_xlfn.IFS(AND(B62&lt;C62, AND(NOT(ISTEXT(B62)), NOT(ISTEXT(C62)))),"OT", AND(B62&gt;C62, AND(NOT(ISTEXT(B62)), NOT(ISTEXT(C62)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>53</v>
       </c>
@@ -2179,12 +2215,12 @@
       <c r="C63">
         <v>79</v>
       </c>
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
+      <c r="D63" t="str" cm="1">
+        <f t="array" ref="D63">_xlfn.IFS(AND(B63&lt;C63, AND(NOT(ISTEXT(B63)), NOT(ISTEXT(C63)))),"OT", AND(B63&gt;C63, AND(NOT(ISTEXT(B63)), NOT(ISTEXT(C63)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -2194,12 +2230,12 @@
       <c r="C64">
         <v>121</v>
       </c>
-      <c r="D64" t="str">
-        <f t="shared" si="0"/>
+      <c r="D64" t="str" cm="1">
+        <f t="array" ref="D64">_xlfn.IFS(AND(B64&lt;C64, AND(NOT(ISTEXT(B64)), NOT(ISTEXT(C64)))),"OT", AND(B64&gt;C64, AND(NOT(ISTEXT(B64)), NOT(ISTEXT(C64)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>58</v>
       </c>
@@ -2209,12 +2245,12 @@
       <c r="C65">
         <v>54.5</v>
       </c>
-      <c r="D65" t="str">
-        <f t="shared" ref="D65:D67" si="1">IF(B65&lt;C65,"OT","ERC")</f>
+      <c r="D65" t="str" cm="1">
+        <f t="array" ref="D65">_xlfn.IFS(AND(B65&lt;C65, AND(NOT(ISTEXT(B65)), NOT(ISTEXT(C65)))),"OT", AND(B65&gt;C65, AND(NOT(ISTEXT(B65)), NOT(ISTEXT(C65)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -2224,12 +2260,12 @@
       <c r="C66">
         <v>104</v>
       </c>
-      <c r="D66" t="str">
-        <f t="shared" si="1"/>
+      <c r="D66" t="str" cm="1">
+        <f t="array" ref="D66">_xlfn.IFS(AND(B66&lt;C66, AND(NOT(ISTEXT(B66)), NOT(ISTEXT(C66)))),"OT", AND(B66&gt;C66, AND(NOT(ISTEXT(B66)), NOT(ISTEXT(C66)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -2239,14 +2275,14 @@
       <c r="C67">
         <v>190</v>
       </c>
-      <c r="D67" t="str">
-        <f t="shared" si="1"/>
+      <c r="D67" t="str" cm="1">
+        <f t="array" ref="D67">_xlfn.IFS(AND(B67&lt;C67, AND(NOT(ISTEXT(B67)), NOT(ISTEXT(C67)))),"OT", AND(B67&gt;C67, AND(NOT(ISTEXT(B67)), NOT(ISTEXT(C67)))), "ERC", TRUE, "N/A")</f>
         <v>OT</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{EFB3B29F-8460-485E-9A7A-D16A554F19F3}">
-    <sortState ref="A2:D67">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D67">
       <sortCondition ref="D1"/>
     </sortState>
   </autoFilter>
@@ -2264,9 +2300,9 @@
       <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2280,7 +2316,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>78</v>
       </c>
@@ -2295,7 +2331,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>79</v>
       </c>
@@ -2310,7 +2346,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -2325,7 +2361,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2340,7 +2376,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2355,7 +2391,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -2370,7 +2406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2385,7 +2421,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2400,7 +2436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2415,7 +2451,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2430,7 +2466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2445,7 +2481,7 @@
         <v>3371</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -2460,7 +2496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2475,7 +2511,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -2490,7 +2526,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -2505,7 +2541,7 @@
         <v>5319</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -2520,7 +2556,7 @@
         <v>5309.5</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2535,7 +2571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2550,7 +2586,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -2565,7 +2601,7 @@
         <v>764.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -2580,7 +2616,7 @@
         <v>2954.5</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -2595,7 +2631,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>30</v>
       </c>
@@ -2610,7 +2646,7 @@
         <v>5326</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>34</v>
       </c>
@@ -2625,7 +2661,7 @@
         <v>1581</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>35</v>
       </c>
@@ -2640,7 +2676,7 @@
         <v>2758</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -2655,7 +2691,7 @@
         <v>408.5</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -2670,7 +2706,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2685,7 +2721,7 @@
         <v>9679</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>42</v>
       </c>
@@ -2700,7 +2736,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>43</v>
       </c>
@@ -2715,7 +2751,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -2730,7 +2766,7 @@
         <v>18.5</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -2745,7 +2781,7 @@
         <v>2860</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -2760,7 +2796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -2775,7 +2811,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2790,7 +2826,7 @@
         <v>169.5</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>51</v>
       </c>
@@ -2805,7 +2841,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>52</v>
       </c>
@@ -2820,7 +2856,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -2835,7 +2871,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>55</v>
       </c>
@@ -2850,7 +2886,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -2865,7 +2901,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -2880,7 +2916,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -2895,7 +2931,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>72</v>
       </c>
@@ -2917,13 +2953,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF24D01-91C4-401F-8722-EA056751A0DD}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -2937,7 +2973,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -2952,7 +2988,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -2967,7 +3003,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -2982,7 +3018,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -2997,7 +3033,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -3012,7 +3048,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -3027,7 +3063,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3042,7 +3078,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -3057,7 +3093,7 @@
         <v>12.5</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -3072,7 +3108,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -3087,7 +3123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>37</v>
       </c>
@@ -3102,7 +3138,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -3117,7 +3153,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>44</v>
       </c>
@@ -3132,7 +3168,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>50</v>
       </c>
@@ -3147,7 +3183,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>53</v>
       </c>
@@ -3162,7 +3198,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -3177,7 +3213,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>58</v>
       </c>
@@ -3192,7 +3228,7 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -3207,7 +3243,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>63</v>
       </c>
@@ -3222,7 +3258,7 @@
         <v>49.5</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>72</v>
       </c>

</xml_diff>